<commit_message>
remove ridgeside valley and update
</commit_message>
<xml_diff>
--- a/Textures/Portraits for Vendors/[CP] Portraits for Vendors/assets/Credits.xlsx
+++ b/Textures/Portraits for Vendors/[CP] Portraits for Vendors/assets/Credits.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\Stardew Valley\Mods\Stardrop Installed Mods\Additions\Portraits for Vendors\[CP] Portraits for Vendors\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F4B1A4-DC82-468A-B845-C91D7F082019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D314C00-B07E-4AEE-9B2B-24B5AF21DAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7F6BED8-1665-4926-9CDA-29768AB6D237}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$7:$E$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$7:$E$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="77">
   <si>
     <t>Asset from</t>
   </si>
@@ -102,9 +102,6 @@
     <t>JojaCashier_Jessie</t>
   </si>
   <si>
-    <t>JojaCashier_Shane</t>
-  </si>
-  <si>
     <t>MagicBoat_Default</t>
   </si>
   <si>
@@ -241,6 +238,27 @@
   </si>
   <si>
     <t>DecorBoat_Cat</t>
+  </si>
+  <si>
+    <t>Casino_Bouncer</t>
+  </si>
+  <si>
+    <t>Casino_Green</t>
+  </si>
+  <si>
+    <t>DesertTrader_RacerGuy</t>
+  </si>
+  <si>
+    <t>DesertTrader_Scholar</t>
+  </si>
+  <si>
+    <t>Crow_Default</t>
+  </si>
+  <si>
+    <t>IslandTrader_Green</t>
+  </si>
+  <si>
+    <t>IslandTrader_Red</t>
   </si>
 </sst>
 </file>
@@ -855,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A337C04-59F4-452C-921B-80F95ACDEDD1}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -875,7 +893,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B1" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -889,7 +907,7 @@
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
@@ -897,7 +915,7 @@
     </row>
     <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -955,14 +973,16 @@
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="18">
-        <v>6480</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="D10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
@@ -974,7 +994,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
@@ -986,19 +1006,19 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>3</v>
+      <c r="D13" s="18">
+        <v>6480</v>
       </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
@@ -1010,55 +1030,55 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>11</v>
+      <c r="D15" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>11</v>
+      <c r="D16" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>11</v>
+      <c r="D17" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>11</v>
+      <c r="D18" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>6</v>
@@ -1070,19 +1090,19 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>3</v>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>6</v>
@@ -1094,31 +1114,31 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>3</v>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>3</v>
+      <c r="D23" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
@@ -1130,7 +1150,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>6</v>
@@ -1142,7 +1162,7 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
@@ -1154,19 +1174,19 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>11</v>
+      <c r="D27" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>6</v>
@@ -1178,7 +1198,7 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>6</v>
@@ -1190,19 +1210,19 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>11</v>
+      <c r="D30" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>6</v>
@@ -1214,33 +1234,31 @@
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>9</v>
+        <v>54</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>9</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>6</v>
@@ -1252,21 +1270,19 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="D35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>6</v>
@@ -1278,7 +1294,7 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>6</v>
@@ -1290,43 +1306,45 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>9</v>
+        <v>58</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>6</v>
@@ -1338,7 +1356,7 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>6</v>
@@ -1350,7 +1368,7 @@
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>6</v>
@@ -1362,31 +1380,31 @@
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="E44" s="4"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="E45" s="4"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>6</v>
@@ -1398,21 +1416,19 @@
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="D47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>6</v>
@@ -1424,7 +1440,7 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>6</v>
@@ -1436,7 +1452,7 @@
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>6</v>
@@ -1448,7 +1464,7 @@
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>6</v>
@@ -1460,7 +1476,7 @@
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>6</v>
@@ -1472,19 +1488,21 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="18">
-        <v>6480</v>
-      </c>
-      <c r="E53" s="4"/>
+      <c r="D53" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>6</v>
@@ -1496,76 +1514,148 @@
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>9</v>
+        <v>64</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E55" s="4"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>9</v>
+        <v>32</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C58" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="18">
+        <v>6480</v>
+      </c>
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D64" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E58" s="4"/>
-    </row>
-    <row r="59" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="10" t="s">
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25"/>
+      <c r="E65" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="B7:E59" xr:uid="{4A337C04-59F4-452C-921B-80F95ACDEDD1}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:E59">
-      <sortCondition ref="B7:B59"/>
+  <autoFilter ref="B7:E65" xr:uid="{4A337C04-59F4-452C-921B-80F95ACDEDD1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:E65">
+      <sortCondition ref="B7:B65"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:B61">
-    <sortCondition ref="B8:B61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:B67">
+    <sortCondition ref="B8:B67"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
@@ -1573,34 +1663,37 @@
     <mergeCell ref="B3:E3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C55" r:id="rId1" display="https://www.nexusmods.com/stardewvalley/mods/3753" xr:uid="{345BDB16-9D9C-4161-AA77-6B3C5843E5CD}"/>
-    <hyperlink ref="C56" r:id="rId2" display="https://www.nexusmods.com/stardewvalley/mods/3753" xr:uid="{F4F96E07-7351-4B47-86FD-89CF75D334EA}"/>
-    <hyperlink ref="C57" r:id="rId3" display="https://www.nexusmods.com/stardewvalley/mods/3753" xr:uid="{95E22557-5EF6-40F1-83E5-0ED908273C51}"/>
-    <hyperlink ref="D12" r:id="rId4" display="https://twitter.com/AndiasRakhman" xr:uid="{E8A8C852-C38B-4573-9381-8E05C2D55CF5}"/>
-    <hyperlink ref="D13" r:id="rId5" display="https://twitter.com/AndiasRakhman" xr:uid="{D80CC328-AFF6-4F18-BA14-7C5B55CA772C}"/>
-    <hyperlink ref="D39" r:id="rId6" display="https://www.nexusmods.com/stardewvalley/users/68088657" xr:uid="{59D88D3C-69C2-469C-B58A-B17DBABA4BCA}"/>
-    <hyperlink ref="C39" r:id="rId7" display="https://www.nexusmods.com/stardewvalley/mods/6398" xr:uid="{7D3AD4D0-14D7-411F-8372-B65B457E91D1}"/>
-    <hyperlink ref="D58" r:id="rId8" display="https://www.nexusmods.com/stardewvalley/users/77325553" xr:uid="{FF583FAE-CF21-4A24-AF69-C3B9A5679743}"/>
-    <hyperlink ref="D55" r:id="rId9" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{C47A5B35-6470-4D17-BC94-6FEEC59B7531}"/>
-    <hyperlink ref="D56" r:id="rId10" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{9663B624-709D-454E-BD48-0EB227AC5F44}"/>
-    <hyperlink ref="D57" r:id="rId11" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{0BA4259C-5F6B-4EED-9222-575FED178246}"/>
-    <hyperlink ref="D47" r:id="rId12" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{03EE9D40-E951-4B20-AB8D-DFFC7044DBBB}"/>
-    <hyperlink ref="C58" r:id="rId13" display="https://www.nexusmods.com/stardewvalley/mods/14916" xr:uid="{8D435C66-17F3-4B7F-93A6-FFB0691B74C7}"/>
-    <hyperlink ref="D38" r:id="rId14" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{5F681CDC-830C-43B4-9E92-77B7A876D199}"/>
-    <hyperlink ref="D59" r:id="rId15" xr:uid="{770B42DE-1C0F-4E30-A07F-FA0DDBC524E2}"/>
-    <hyperlink ref="C38" r:id="rId16" display="https://www.nexusmods.com/stardewvalley/mods/3753" xr:uid="{B8D74AD2-CFFA-4A91-BCE6-7410CFC11512}"/>
-    <hyperlink ref="D20" r:id="rId17" display="https://twitter.com/AndiasRakhman" xr:uid="{E17B9340-DAA4-4E60-BF80-8B85D57F81E7}"/>
-    <hyperlink ref="D22" r:id="rId18" display="https://twitter.com/AndiasRakhman" xr:uid="{F911FD76-C29D-443A-B31A-6197E2EA8EC5}"/>
-    <hyperlink ref="D23" r:id="rId19" display="https://twitter.com/AndiasRakhman" xr:uid="{A93C98E3-B69A-4DC3-9B6F-282FE7D11D41}"/>
-    <hyperlink ref="D25" r:id="rId20" display="https://twitter.com/AndiasRakhman" xr:uid="{90281A66-9AAC-4340-9350-F56241842143}"/>
-    <hyperlink ref="D35" r:id="rId21" display="https://www.nexusmods.com/stardewvalley/mods/3753" xr:uid="{2E111352-E23C-4408-9B0A-EB8857D14E92}"/>
-    <hyperlink ref="D32" r:id="rId22" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{71FF429F-E212-46C1-BFD8-3312F128B841}"/>
-    <hyperlink ref="E33" r:id="rId23" display="https://twitter.com/AndiasRakhman" xr:uid="{AD854E10-72F7-4750-AC9D-EF50E585A7FE}"/>
-    <hyperlink ref="D28" r:id="rId24" display="https://twitter.com/AndiasRakhman" xr:uid="{06FCD8EB-D322-4918-86FE-668E7998B507}"/>
-    <hyperlink ref="D10" r:id="rId25" display="https://www.nexusmods.com/stardewvalley/users/55537262" xr:uid="{01696168-25AC-4DC6-8F68-12999FEBAC6E}"/>
-    <hyperlink ref="D53" r:id="rId26" display="https://www.nexusmods.com/stardewvalley/users/55537262" xr:uid="{3779AC8C-EA1F-43BD-9FC0-D0567FD97F16}"/>
+    <hyperlink ref="C61" r:id="rId1" display="https://www.nexusmods.com/stardewvalley/mods/3753" xr:uid="{345BDB16-9D9C-4161-AA77-6B3C5843E5CD}"/>
+    <hyperlink ref="C62" r:id="rId2" display="https://www.nexusmods.com/stardewvalley/mods/3753" xr:uid="{F4F96E07-7351-4B47-86FD-89CF75D334EA}"/>
+    <hyperlink ref="C63" r:id="rId3" display="https://www.nexusmods.com/stardewvalley/mods/3753" xr:uid="{95E22557-5EF6-40F1-83E5-0ED908273C51}"/>
+    <hyperlink ref="D15" r:id="rId4" display="https://twitter.com/AndiasRakhman" xr:uid="{E8A8C852-C38B-4573-9381-8E05C2D55CF5}"/>
+    <hyperlink ref="D16" r:id="rId5" display="https://twitter.com/AndiasRakhman" xr:uid="{D80CC328-AFF6-4F18-BA14-7C5B55CA772C}"/>
+    <hyperlink ref="D45" r:id="rId6" display="https://www.nexusmods.com/stardewvalley/users/68088657" xr:uid="{59D88D3C-69C2-469C-B58A-B17DBABA4BCA}"/>
+    <hyperlink ref="C45" r:id="rId7" display="https://www.nexusmods.com/stardewvalley/mods/6398" xr:uid="{7D3AD4D0-14D7-411F-8372-B65B457E91D1}"/>
+    <hyperlink ref="D64" r:id="rId8" display="https://www.nexusmods.com/stardewvalley/users/77325553" xr:uid="{FF583FAE-CF21-4A24-AF69-C3B9A5679743}"/>
+    <hyperlink ref="D61" r:id="rId9" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{C47A5B35-6470-4D17-BC94-6FEEC59B7531}"/>
+    <hyperlink ref="D62" r:id="rId10" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{9663B624-709D-454E-BD48-0EB227AC5F44}"/>
+    <hyperlink ref="D63" r:id="rId11" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{0BA4259C-5F6B-4EED-9222-575FED178246}"/>
+    <hyperlink ref="D53" r:id="rId12" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{03EE9D40-E951-4B20-AB8D-DFFC7044DBBB}"/>
+    <hyperlink ref="C64" r:id="rId13" display="https://www.nexusmods.com/stardewvalley/mods/14916" xr:uid="{8D435C66-17F3-4B7F-93A6-FFB0691B74C7}"/>
+    <hyperlink ref="D44" r:id="rId14" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{5F681CDC-830C-43B4-9E92-77B7A876D199}"/>
+    <hyperlink ref="D65" r:id="rId15" xr:uid="{770B42DE-1C0F-4E30-A07F-FA0DDBC524E2}"/>
+    <hyperlink ref="C44" r:id="rId16" display="https://www.nexusmods.com/stardewvalley/mods/3753" xr:uid="{B8D74AD2-CFFA-4A91-BCE6-7410CFC11512}"/>
+    <hyperlink ref="D25" r:id="rId17" display="https://twitter.com/AndiasRakhman" xr:uid="{E17B9340-DAA4-4E60-BF80-8B85D57F81E7}"/>
+    <hyperlink ref="D27" r:id="rId18" display="https://twitter.com/AndiasRakhman" xr:uid="{F911FD76-C29D-443A-B31A-6197E2EA8EC5}"/>
+    <hyperlink ref="D28" r:id="rId19" display="https://twitter.com/AndiasRakhman" xr:uid="{A93C98E3-B69A-4DC3-9B6F-282FE7D11D41}"/>
+    <hyperlink ref="D30" r:id="rId20" display="https://twitter.com/AndiasRakhman" xr:uid="{90281A66-9AAC-4340-9350-F56241842143}"/>
+    <hyperlink ref="D39" r:id="rId21" display="https://www.nexusmods.com/stardewvalley/users/2679113" xr:uid="{71FF429F-E212-46C1-BFD8-3312F128B841}"/>
+    <hyperlink ref="E40" r:id="rId22" display="https://twitter.com/AndiasRakhman" xr:uid="{AD854E10-72F7-4750-AC9D-EF50E585A7FE}"/>
+    <hyperlink ref="D33" r:id="rId23" display="https://twitter.com/AndiasRakhman" xr:uid="{06FCD8EB-D322-4918-86FE-668E7998B507}"/>
+    <hyperlink ref="D13" r:id="rId24" display="https://www.nexusmods.com/stardewvalley/users/55537262" xr:uid="{01696168-25AC-4DC6-8F68-12999FEBAC6E}"/>
+    <hyperlink ref="D59" r:id="rId25" display="https://www.nexusmods.com/stardewvalley/users/55537262" xr:uid="{3779AC8C-EA1F-43BD-9FC0-D0567FD97F16}"/>
+    <hyperlink ref="D10" r:id="rId26" display="https://www.nexusmods.com/stardewvalley/mods/3753" xr:uid="{0D69D8D0-E2B7-4D4B-BC59-DACE18EBAB81}"/>
+    <hyperlink ref="D17" r:id="rId27" display="https://twitter.com/AndiasRakhman" xr:uid="{F192F78A-BCCD-4E8E-8DF3-F4552069D2E1}"/>
+    <hyperlink ref="D18" r:id="rId28" display="https://twitter.com/AndiasRakhman" xr:uid="{957294D4-AD3D-4E3C-A67E-EAF0BD32D069}"/>
+    <hyperlink ref="D12" r:id="rId29" display="https://twitter.com/AndiasRakhman" xr:uid="{281AD3BF-9BF0-4ABB-B9D1-B0BF14649998}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>